<commit_message>
Commit 02: Team 10 Finish 2nd Progress
Co-Authored-By: trunghiencdr <60185219+trunghiencdr@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Nhom10_ProjectPlan.xlsx
+++ b/Nhom10_ProjectPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>TT</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Xong</t>
+  </si>
+  <si>
+    <t>Hien</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -288,6 +291,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -726,34 +735,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -881,8 +890,12 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,8 +907,12 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,8 +924,12 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -920,8 +941,12 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,8 +958,12 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -946,8 +975,12 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -959,8 +992,12 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -972,8 +1009,12 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,8 +1026,12 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,8 +1056,12 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1024,8 +1073,12 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1037,8 +1090,12 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,8 +1107,12 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,8 +1124,12 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,8 +1141,12 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,8 +1158,12 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1102,8 +1175,12 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 07: Finish Customer Layout
</commit_message>
<xml_diff>
--- a/Nhom10_ProjectPlan.xlsx
+++ b/Nhom10_ProjectPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>TT</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Xong</t>
+  </si>
+  <si>
+    <t>Hien</t>
   </si>
 </sst>
 </file>
@@ -710,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -881,7 +884,9 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -894,7 +899,9 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -907,7 +914,9 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
@@ -920,7 +929,9 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
@@ -933,7 +944,9 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
@@ -946,7 +959,9 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
@@ -959,7 +974,9 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
@@ -972,7 +989,9 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
@@ -985,7 +1004,9 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>

</xml_diff>

<commit_message>
Commit 08: Add Folder And Second Chap
</commit_message>
<xml_diff>
--- a/Nhom10_ProjectPlan.xlsx
+++ b/Nhom10_ProjectPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>TT</t>
   </si>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +291,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -713,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,34 +732,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -887,7 +890,9 @@
       <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -902,7 +907,9 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,7 +924,9 @@
       <c r="E14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -932,7 +941,9 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -947,7 +958,9 @@
       <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -962,7 +975,9 @@
       <c r="E17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -977,7 +992,9 @@
       <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,7 +1009,9 @@
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1007,7 +1026,9 @@
       <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 03: Team 10 Finish 3rd and 4st Progress
</commit_message>
<xml_diff>
--- a/Nhom10_ProjectPlan.xlsx
+++ b/Nhom10_ProjectPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>TT</t>
   </si>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +291,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -719,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -735,34 +738,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1205,8 +1208,12 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1218,8 +1225,12 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1231,8 +1242,12 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Team 10 Final Doc Commit
</commit_message>
<xml_diff>
--- a/Nhom10_ProjectPlan.xlsx
+++ b/Nhom10_ProjectPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>TT</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Hien</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Long + Hien</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +294,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -716,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,34 +738,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1053,8 +1059,12 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,8 +1076,12 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,8 +1093,12 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1092,8 +1110,12 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1105,8 +1127,12 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,8 +1144,12 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1131,8 +1161,12 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1144,8 +1178,12 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1170,8 +1208,12 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,8 +1225,12 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1196,8 +1242,12 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1235,8 +1285,12 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="G36" s="1"/>
     </row>
   </sheetData>

</xml_diff>